<commit_message>
Reorder first two weeks of material
</commit_message>
<xml_diff>
--- a/course-admin/schedule.xlsx
+++ b/course-admin/schedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soltoffbc/Projects/Math and Statistics/fall-course/css18.github.io/course_admin/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soltoffbc/Projects/Math and Statistics/fall-course/css18.github.io/course-admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA56BAA5-F7D6-CE45-857D-4E9E67EF9563}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA6892E8-C3F5-8D4D-8E41-7A910F287198}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="440" yWindow="760" windowWidth="21240" windowHeight="15940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -111,9 +111,6 @@
     <t>Data visualizations</t>
   </si>
   <si>
-    <t>Grammar of graphics and `ggplot2`</t>
-  </si>
-  <si>
     <t>Probability</t>
   </si>
   <si>
@@ -157,6 +154,9 @@
   </si>
   <si>
     <t>OLS - multivariable/interaction terms</t>
+  </si>
+  <si>
+    <t>Visualizations and the grammar of graphics</t>
   </si>
 </sst>
 </file>
@@ -479,7 +479,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C21"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -510,7 +510,7 @@
         <v>43374</v>
       </c>
       <c r="C2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
         <v>24</v>
@@ -528,7 +528,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -558,7 +558,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -573,7 +573,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -588,7 +588,7 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -603,7 +603,7 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -618,7 +618,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -633,7 +633,7 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -648,7 +648,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -663,7 +663,7 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -678,7 +678,7 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -693,7 +693,7 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -708,7 +708,7 @@
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -723,7 +723,7 @@
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -738,7 +738,7 @@
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -753,7 +753,7 @@
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -768,7 +768,7 @@
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -783,7 +783,7 @@
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -798,7 +798,7 @@
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rename cm003 to Graphical Data Analysis
</commit_message>
<xml_diff>
--- a/course-admin/schedule.xlsx
+++ b/course-admin/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soltoffbc/Projects/Math and Statistics/fall-course/css18.github.io/course-admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA6892E8-C3F5-8D4D-8E41-7A910F287198}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25615DFB-33BD-684D-A943-8B4A97799072}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="440" yWindow="760" windowWidth="21240" windowHeight="15940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -108,9 +108,6 @@
     <t>Data objects/tidy data</t>
   </si>
   <si>
-    <t>Data visualizations</t>
-  </si>
-  <si>
     <t>Probability</t>
   </si>
   <si>
@@ -157,6 +154,9 @@
   </si>
   <si>
     <t>Visualizations and the grammar of graphics</t>
+  </si>
+  <si>
+    <t>Graphical data analysis</t>
   </si>
 </sst>
 </file>
@@ -479,7 +479,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -528,7 +528,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -543,7 +543,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -573,7 +573,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -588,7 +588,7 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -603,7 +603,7 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -618,7 +618,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -633,7 +633,7 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -648,7 +648,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -663,7 +663,7 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -678,7 +678,7 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -693,7 +693,7 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -708,7 +708,7 @@
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -723,7 +723,7 @@
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -738,7 +738,7 @@
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -753,7 +753,7 @@
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -768,7 +768,7 @@
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -783,7 +783,7 @@
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -798,7 +798,7 @@
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add link to cm002 to the syllabus
</commit_message>
<xml_diff>
--- a/course-admin/schedule.xlsx
+++ b/course-admin/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soltoffbc/Projects/Math and Statistics/fall-course/css18.github.io/course-admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25615DFB-33BD-684D-A943-8B4A97799072}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{962ADB2C-7676-1D4C-BCDB-42F7EA50ACFA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="440" yWindow="760" windowWidth="21240" windowHeight="15940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -479,7 +479,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -525,7 +525,7 @@
         <v>43376</v>
       </c>
       <c r="C3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Revise titles for week 4 topics
</commit_message>
<xml_diff>
--- a/course-admin/schedule.xlsx
+++ b/course-admin/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soltoffbc/Projects/Math and Statistics/fall-course/css18.github.io/course-admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB72CB9B-D64A-4847-87BA-68353A4BDCED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BED392-0CB5-DD4E-9198-628E88F838F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="440" yWindow="760" windowWidth="21240" windowHeight="15940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -111,12 +111,6 @@
     <t>Probability</t>
   </si>
   <si>
-    <t>Random variables</t>
-  </si>
-  <si>
-    <t>Simulating random variables</t>
-  </si>
-  <si>
     <t>Expectation</t>
   </si>
   <si>
@@ -157,6 +151,12 @@
   </si>
   <si>
     <t>Functions and iterative operations</t>
+  </si>
+  <si>
+    <t>Discrete random variables</t>
+  </si>
+  <si>
+    <t>Continuous random variables</t>
   </si>
 </sst>
 </file>
@@ -479,7 +479,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -528,7 +528,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -543,7 +543,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -588,7 +588,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -603,7 +603,7 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -618,7 +618,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -633,7 +633,7 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -648,7 +648,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -663,7 +663,7 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -678,7 +678,7 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -693,7 +693,7 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -708,7 +708,7 @@
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -723,7 +723,7 @@
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -738,7 +738,7 @@
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -753,7 +753,7 @@
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -768,7 +768,7 @@
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -783,7 +783,7 @@
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -798,7 +798,7 @@
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Spread random variables across two weeks - integrate expectation into the discussion of each kind of random variable
</commit_message>
<xml_diff>
--- a/course-admin/schedule.xlsx
+++ b/course-admin/schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11015"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soltoffbc/Projects/Math and Statistics/fall-course/css18.github.io/course-admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BED392-0CB5-DD4E-9198-628E88F838F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD78ECF-5E5C-D147-97B7-BF46A272F78A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="440" yWindow="760" windowWidth="21240" windowHeight="15940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
   <si>
     <t>topic</t>
   </si>
@@ -109,12 +109,6 @@
   </si>
   <si>
     <t>Probability</t>
-  </si>
-  <si>
-    <t>Expectation</t>
-  </si>
-  <si>
-    <t>Convergence</t>
   </si>
   <si>
     <t>Parametric inference</t>
@@ -479,7 +473,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -528,7 +522,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -543,7 +537,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -588,7 +582,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -603,7 +597,7 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -618,7 +612,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -633,7 +627,7 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -648,7 +642,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -663,7 +657,7 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -678,7 +672,7 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -693,7 +687,7 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -708,7 +702,7 @@
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -723,7 +717,7 @@
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -738,7 +732,7 @@
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -753,7 +747,7 @@
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -768,7 +762,7 @@
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -783,7 +777,7 @@
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -798,7 +792,7 @@
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add cm008 to the syllabus
</commit_message>
<xml_diff>
--- a/course-admin/schedule.xlsx
+++ b/course-admin/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soltoffbc/Projects/Math and Statistics/fall-course/css18.github.io/course-admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08389B4C-BA52-1E49-95F3-4BA48537F17F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C965E73-5783-344D-B31B-A112C5EBAF14}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="440" yWindow="760" windowWidth="21240" windowHeight="15940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>topic</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>Continuous random variables</t>
+  </si>
+  <si>
+    <t>Discrete random variables in R</t>
   </si>
 </sst>
 </file>
@@ -473,7 +476,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -609,10 +612,10 @@
         <v>43397</v>
       </c>
       <c r="C9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add cm010 and fix the dates on the syllabus
</commit_message>
<xml_diff>
--- a/course-admin/schedule.xlsx
+++ b/course-admin/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soltoffbc/Projects/Math and Statistics/fall-course/css18.github.io/course-admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C965E73-5783-344D-B31B-A112C5EBAF14}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C653FC7F-2BFA-2A48-96D7-235D62B466F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="440" yWindow="760" windowWidth="21240" windowHeight="15940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -476,7 +476,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -504,7 +504,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2">
-        <v>43374</v>
+        <v>43375</v>
       </c>
       <c r="C2" s="2" t="b">
         <v>1</v>
@@ -519,7 +519,7 @@
       </c>
       <c r="B3" s="2">
         <f>B2+2</f>
-        <v>43376</v>
+        <v>43377</v>
       </c>
       <c r="C3" s="2" t="b">
         <v>1</v>
@@ -534,7 +534,7 @@
       </c>
       <c r="B4" s="2">
         <f>B2+7</f>
-        <v>43381</v>
+        <v>43382</v>
       </c>
       <c r="C4" s="2" t="b">
         <v>1</v>
@@ -549,7 +549,7 @@
       </c>
       <c r="B5" s="2">
         <f t="shared" ref="B5" si="0">B4+2</f>
-        <v>43383</v>
+        <v>43384</v>
       </c>
       <c r="C5" s="2" t="b">
         <v>1</v>
@@ -564,7 +564,7 @@
       </c>
       <c r="B6" s="2">
         <f t="shared" ref="B6" si="1">B4+7</f>
-        <v>43388</v>
+        <v>43389</v>
       </c>
       <c r="C6" s="2" t="b">
         <v>1</v>
@@ -579,7 +579,7 @@
       </c>
       <c r="B7" s="2">
         <f t="shared" ref="B7" si="2">B6+2</f>
-        <v>43390</v>
+        <v>43391</v>
       </c>
       <c r="C7" s="2" t="b">
         <v>1</v>
@@ -594,7 +594,7 @@
       </c>
       <c r="B8" s="2">
         <f t="shared" ref="B8" si="3">B6+7</f>
-        <v>43395</v>
+        <v>43396</v>
       </c>
       <c r="C8" s="2" t="b">
         <v>1</v>
@@ -609,7 +609,7 @@
       </c>
       <c r="B9" s="2">
         <f t="shared" ref="B9" si="4">B8+2</f>
-        <v>43397</v>
+        <v>43398</v>
       </c>
       <c r="C9" s="2" t="b">
         <v>1</v>
@@ -624,7 +624,7 @@
       </c>
       <c r="B10" s="2">
         <f t="shared" ref="B10" si="5">B8+7</f>
-        <v>43402</v>
+        <v>43403</v>
       </c>
       <c r="C10" s="2" t="b">
         <v>0</v>
@@ -639,10 +639,10 @@
       </c>
       <c r="B11" s="2">
         <f t="shared" ref="B11" si="6">B10+2</f>
-        <v>43404</v>
+        <v>43405</v>
       </c>
       <c r="C11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" t="s">
         <v>40</v>
@@ -654,7 +654,7 @@
       </c>
       <c r="B12" s="2">
         <f t="shared" ref="B12" si="7">B10+7</f>
-        <v>43409</v>
+        <v>43410</v>
       </c>
       <c r="C12" s="2" t="b">
         <v>0</v>
@@ -669,7 +669,7 @@
       </c>
       <c r="B13" s="2">
         <f t="shared" ref="B13" si="8">B12+2</f>
-        <v>43411</v>
+        <v>43412</v>
       </c>
       <c r="C13" s="2" t="b">
         <v>0</v>
@@ -684,7 +684,7 @@
       </c>
       <c r="B14" s="2">
         <f t="shared" ref="B14" si="9">B12+7</f>
-        <v>43416</v>
+        <v>43417</v>
       </c>
       <c r="C14" s="2" t="b">
         <v>0</v>
@@ -699,7 +699,7 @@
       </c>
       <c r="B15" s="2">
         <f t="shared" ref="B15" si="10">B14+2</f>
-        <v>43418</v>
+        <v>43419</v>
       </c>
       <c r="C15" s="2" t="b">
         <v>0</v>
@@ -714,7 +714,7 @@
       </c>
       <c r="B16" s="2">
         <f t="shared" ref="B16" si="11">B14+7</f>
-        <v>43423</v>
+        <v>43424</v>
       </c>
       <c r="C16" s="2" t="b">
         <v>0</v>
@@ -729,7 +729,7 @@
       </c>
       <c r="B17" s="2">
         <f t="shared" ref="B17" si="12">B16+2</f>
-        <v>43425</v>
+        <v>43426</v>
       </c>
       <c r="C17" s="2" t="b">
         <v>0</v>
@@ -744,7 +744,7 @@
       </c>
       <c r="B18" s="2">
         <f t="shared" ref="B18" si="13">B16+7</f>
-        <v>43430</v>
+        <v>43431</v>
       </c>
       <c r="C18" s="2" t="b">
         <v>0</v>
@@ -759,7 +759,7 @@
       </c>
       <c r="B19" s="2">
         <f t="shared" ref="B19" si="14">B18+2</f>
-        <v>43432</v>
+        <v>43433</v>
       </c>
       <c r="C19" s="2" t="b">
         <v>0</v>
@@ -774,7 +774,7 @@
       </c>
       <c r="B20" s="2">
         <f t="shared" ref="B20" si="15">B18+7</f>
-        <v>43437</v>
+        <v>43438</v>
       </c>
       <c r="C20" s="2" t="b">
         <v>0</v>
@@ -789,7 +789,7 @@
       </c>
       <c r="B21" s="2">
         <f t="shared" ref="B21" si="16">B20+2</f>
-        <v>43439</v>
+        <v>43440</v>
       </c>
       <c r="C21" s="2" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Fix the schedule due to the plague week
</commit_message>
<xml_diff>
--- a/course-admin/schedule.xlsx
+++ b/course-admin/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soltoffbc/Projects/Math and Statistics/fall-course/css18.github.io/course-admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C653FC7F-2BFA-2A48-96D7-235D62B466F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E59D394C-2F64-C643-8EB6-399B2AE0D4FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="440" yWindow="760" windowWidth="21240" windowHeight="15940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -114,15 +114,6 @@
     <t>Parametric inference</t>
   </si>
   <si>
-    <t>Functions/optimization in R</t>
-  </si>
-  <si>
-    <t>Hypothesis testing</t>
-  </si>
-  <si>
-    <t>Hypothesis testing in R</t>
-  </si>
-  <si>
     <t>Bayesian inference</t>
   </si>
   <si>
@@ -154,6 +145,15 @@
   </si>
   <si>
     <t>Discrete random variables in R</t>
+  </si>
+  <si>
+    <t>Class canceled - sickness</t>
+  </si>
+  <si>
+    <t>Optimization</t>
+  </si>
+  <si>
+    <t>Parametric inference in R</t>
   </si>
 </sst>
 </file>
@@ -476,7 +476,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -525,7 +525,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -540,7 +540,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -585,7 +585,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -600,7 +600,7 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -615,7 +615,7 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -630,7 +630,7 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -642,10 +642,10 @@
         <v>43405</v>
       </c>
       <c r="C11" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -660,7 +660,7 @@
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -675,7 +675,7 @@
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -690,7 +690,7 @@
         <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -705,7 +705,7 @@
         <v>0</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -720,7 +720,7 @@
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -735,7 +735,7 @@
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -750,7 +750,7 @@
         <v>0</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -765,7 +765,7 @@
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -780,7 +780,7 @@
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -795,7 +795,7 @@
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update and activate cm011
</commit_message>
<xml_diff>
--- a/course-admin/schedule.xlsx
+++ b/course-admin/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soltoffbc/Projects/Math and Statistics/fall-course/css18.github.io/course-admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E59D394C-2F64-C643-8EB6-399B2AE0D4FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDFE2077-7E05-A94F-8464-B120DF0D4F41}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="440" yWindow="760" windowWidth="21240" windowHeight="15940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -476,7 +476,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -657,7 +657,7 @@
         <v>43410</v>
       </c>
       <c r="C12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
Add cm012 to the syllabus
</commit_message>
<xml_diff>
--- a/course-admin/schedule.xlsx
+++ b/course-admin/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soltoffbc/Projects/Math and Statistics/fall-course/css18.github.io/course-admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDFE2077-7E05-A94F-8464-B120DF0D4F41}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E351EE3-75EF-004C-A04C-04C7C6ABD129}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="440" yWindow="760" windowWidth="21240" windowHeight="15940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -476,7 +476,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -672,7 +672,7 @@
         <v>43412</v>
       </c>
       <c r="C13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Add cm014 to syllabus
</commit_message>
<xml_diff>
--- a/course-admin/schedule.xlsx
+++ b/course-admin/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soltoffbc/Projects/Math and Statistics/fall-course/css18.github.io/course-admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDA42ED-AB81-E543-BD43-ABF8F3558F82}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CA9F964-EDF8-3A45-B326-2B1B26626B90}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="440" yWindow="760" windowWidth="21240" windowHeight="15940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -479,7 +479,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -690,7 +690,7 @@
         <v>43417</v>
       </c>
       <c r="C14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" t="s">
         <v>40</v>
@@ -705,7 +705,7 @@
         <v>43419</v>
       </c>
       <c r="C15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Update syllabus for OLS
</commit_message>
<xml_diff>
--- a/course-admin/schedule.xlsx
+++ b/course-admin/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soltoffbc/Projects/Math and Statistics/fall-course/css18.github.io/course-admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BC86F83-9EDB-8E42-ADA1-A271F0C16ACE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81911CCB-144C-4940-9FC2-2612A2D4706A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="440" yWindow="760" windowWidth="21240" windowHeight="15940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -117,15 +117,6 @@
     <t>Bayesian inference</t>
   </si>
   <si>
-    <t>OLS - properties of estimators</t>
-  </si>
-  <si>
-    <t>OLS - interpretation/hypothesis testing</t>
-  </si>
-  <si>
-    <t>OLS - multivariable/interaction terms</t>
-  </si>
-  <si>
     <t>Visualizations and the grammar of graphics</t>
   </si>
   <si>
@@ -157,6 +148,15 @@
   </si>
   <si>
     <t>Hypothesis testing</t>
+  </si>
+  <si>
+    <t>Ordinary least squares - foundation and diagnostics</t>
+  </si>
+  <si>
+    <t>Ordinary least squares - interpretation/hypothesis testing</t>
+  </si>
+  <si>
+    <t>Ordinary least squares - multivariable/interaction terms</t>
   </si>
 </sst>
 </file>
@@ -479,7 +479,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -528,7 +528,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -543,7 +543,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -588,7 +588,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -603,7 +603,7 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -618,7 +618,7 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -633,7 +633,7 @@
         <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -648,7 +648,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -663,7 +663,7 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -678,7 +678,7 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -693,7 +693,7 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -723,7 +723,7 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -738,7 +738,7 @@
         <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -768,7 +768,7 @@
         <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -783,7 +783,7 @@
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -798,7 +798,7 @@
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add cm018 to syllabus
</commit_message>
<xml_diff>
--- a/course-admin/schedule.xlsx
+++ b/course-admin/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soltoffbc/Projects/Math and Statistics/fall-course/css18.github.io/course-admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81911CCB-144C-4940-9FC2-2612A2D4706A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6788BD40-A522-4E45-88F3-76DAFD2A3AD1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="440" yWindow="760" windowWidth="21240" windowHeight="15940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -479,7 +479,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -765,7 +765,7 @@
         <v>43433</v>
       </c>
       <c r="C19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
Add cm019 to syllabus
</commit_message>
<xml_diff>
--- a/course-admin/schedule.xlsx
+++ b/course-admin/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soltoffbc/Projects/Math and Statistics/fall-course/css18.github.io/course-admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6788BD40-A522-4E45-88F3-76DAFD2A3AD1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D3B904-C9CB-2747-A018-5FD5068DDF21}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="440" yWindow="760" windowWidth="21240" windowHeight="15940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -479,7 +479,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -780,7 +780,7 @@
         <v>43438</v>
       </c>
       <c r="C20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
Add cm020 to syllabus
</commit_message>
<xml_diff>
--- a/course-admin/schedule.xlsx
+++ b/course-admin/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/soltoffbc/Projects/Math and Statistics/fall-course/css18.github.io/course-admin/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D3B904-C9CB-2747-A018-5FD5068DDF21}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96104404-6B05-A941-B945-51A562F05FCE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="440" yWindow="760" windowWidth="21240" windowHeight="15940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -479,7 +479,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -795,7 +795,7 @@
         <v>43440</v>
       </c>
       <c r="C21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" t="s">
         <v>42</v>

</xml_diff>